<commit_message>
update asrt_percept and asrt_motor to fix feedback related errors
</commit_message>
<xml_diff>
--- a/asrt_motor/sequences/learning_sequence_file_list.xlsx
+++ b/asrt_motor/sequences/learning_sequence_file_list.xlsx
@@ -443,140 +443,140 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>sequences/867746_learning_sequence_00.csv</t>
+          <t>sequences/278857_learning_sequence_00.csv</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>sequences/867746_learning_sequence_01.csv</t>
+          <t>sequences/278857_learning_sequence_01.csv</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>sequences/867746_learning_sequence_02.csv</t>
+          <t>sequences/278857_learning_sequence_02.csv</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>sequences/867746_learning_sequence_03.csv</t>
+          <t>sequences/278857_learning_sequence_03.csv</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>sequences/867746_learning_sequence_04.csv</t>
+          <t>sequences/278857_learning_sequence_04.csv</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>sequences/867746_learning_sequence_05.csv</t>
+          <t>sequences/278857_learning_sequence_05.csv</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>sequences/867746_learning_sequence_06.csv</t>
+          <t>sequences/278857_learning_sequence_06.csv</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>sequences/867746_learning_sequence_07.csv</t>
+          <t>sequences/278857_learning_sequence_07.csv</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>sequences/867746_learning_sequence_08.csv</t>
+          <t>sequences/278857_learning_sequence_08.csv</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>sequences/867746_learning_sequence_09.csv</t>
+          <t>sequences/278857_learning_sequence_09.csv</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>sequences/867746_learning_sequence_10.csv</t>
+          <t>sequences/278857_learning_sequence_10.csv</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>sequences/867746_learning_sequence_11.csv</t>
+          <t>sequences/278857_learning_sequence_11.csv</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>sequences/867746_learning_sequence_12.csv</t>
+          <t>sequences/278857_learning_sequence_12.csv</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>sequences/867746_learning_sequence_13.csv</t>
+          <t>sequences/278857_learning_sequence_13.csv</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>sequences/867746_learning_sequence_14.csv</t>
+          <t>sequences/278857_learning_sequence_14.csv</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>sequences/867746_learning_sequence_15.csv</t>
+          <t>sequences/278857_learning_sequence_15.csv</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>sequences/867746_learning_sequence_16.csv</t>
+          <t>sequences/278857_learning_sequence_16.csv</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>sequences/867746_learning_sequence_17.csv</t>
+          <t>sequences/278857_learning_sequence_17.csv</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>sequences/867746_learning_sequence_18.csv</t>
+          <t>sequences/278857_learning_sequence_18.csv</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>sequences/867746_learning_sequence_19.csv</t>
+          <t>sequences/278857_learning_sequence_19.csv</t>
         </is>
       </c>
     </row>

</xml_diff>